<commit_message>
Analysis_script.jl finally formats data correctly, moving on to actual analysis
</commit_message>
<xml_diff>
--- a/Research Project Data File.xlsx
+++ b/Research Project Data File.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/04cde3730d8bf776/Documents/Uni Docs/STAT1301 2- Electric Boogaloo/Research Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ec892e7e4853af95/Documents/UNI/UNI 1 SEM 2/STAT1301/Research/Arthur-s-STAT1301-Project-on-Valerian-Root/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="509" documentId="8_{9311CA3D-7FF6-4128-B46A-1A9324E1D225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC7D8CA1-83A3-4CC6-8415-2E1AB670CF86}"/>
+  <xr:revisionPtr revIDLastSave="528" documentId="8_{9311CA3D-7FF6-4128-B46A-1A9324E1D225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{932F8BC7-AE1F-4CD6-925E-38BF3873E2AA}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="10530" yWindow="2550" windowWidth="8670" windowHeight="9450" xr2:uid="{B1D913C5-7F24-403E-865C-599D1658A181}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B1D913C5-7F24-403E-865C-599D1658A181}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="83">
   <si>
     <t>Subject Name</t>
   </si>
@@ -292,6 +293,12 @@
   <si>
     <t>Age (years)</t>
   </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
 </sst>
 </file>
 
@@ -446,6 +453,7 @@
                   <c:y val="-0.10143518518518518"/>
                 </c:manualLayout>
               </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -3394,10 +3402,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3714,32 +3718,1510 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB63271F-69B0-4854-9623-6BAC9B90FB1F}">
+  <dimension ref="A1:G63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="16" max="16" width="16.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>90</v>
+      </c>
+      <c r="D2">
+        <v>120</v>
+      </c>
+      <c r="E2">
+        <v>105</v>
+      </c>
+      <c r="F2">
+        <v>175</v>
+      </c>
+      <c r="G2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>110</v>
+      </c>
+      <c r="D3">
+        <v>110</v>
+      </c>
+      <c r="E3">
+        <v>95</v>
+      </c>
+      <c r="F3">
+        <v>130</v>
+      </c>
+      <c r="G3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>155</v>
+      </c>
+      <c r="D4">
+        <v>170</v>
+      </c>
+      <c r="E4">
+        <v>145</v>
+      </c>
+      <c r="F4">
+        <v>155</v>
+      </c>
+      <c r="G4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>150</v>
+      </c>
+      <c r="D5">
+        <v>155</v>
+      </c>
+      <c r="E5">
+        <v>105</v>
+      </c>
+      <c r="F5">
+        <v>90</v>
+      </c>
+      <c r="G5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>120</v>
+      </c>
+      <c r="D6">
+        <v>125</v>
+      </c>
+      <c r="E6">
+        <v>55</v>
+      </c>
+      <c r="F6">
+        <v>55</v>
+      </c>
+      <c r="G6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>75</v>
+      </c>
+      <c r="D7">
+        <v>110</v>
+      </c>
+      <c r="E7">
+        <v>120</v>
+      </c>
+      <c r="F7">
+        <v>85</v>
+      </c>
+      <c r="G7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>90</v>
+      </c>
+      <c r="D8">
+        <v>85</v>
+      </c>
+      <c r="E8">
+        <v>65</v>
+      </c>
+      <c r="F8">
+        <v>75</v>
+      </c>
+      <c r="G8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>140</v>
+      </c>
+      <c r="D9">
+        <v>120</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>110</v>
+      </c>
+      <c r="G9">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>175</v>
+      </c>
+      <c r="D10">
+        <v>140</v>
+      </c>
+      <c r="E10">
+        <v>160</v>
+      </c>
+      <c r="F10">
+        <v>155</v>
+      </c>
+      <c r="G10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>120</v>
+      </c>
+      <c r="D11">
+        <v>85</v>
+      </c>
+      <c r="E11">
+        <v>130</v>
+      </c>
+      <c r="F11">
+        <v>115</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>150</v>
+      </c>
+      <c r="D12">
+        <v>180</v>
+      </c>
+      <c r="E12">
+        <v>130</v>
+      </c>
+      <c r="F12">
+        <v>165</v>
+      </c>
+      <c r="G12">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>170</v>
+      </c>
+      <c r="D13">
+        <v>155</v>
+      </c>
+      <c r="E13">
+        <v>110</v>
+      </c>
+      <c r="F13">
+        <v>135</v>
+      </c>
+      <c r="G13">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>150</v>
+      </c>
+      <c r="D14">
+        <v>110</v>
+      </c>
+      <c r="E14">
+        <v>125</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>75</v>
+      </c>
+      <c r="D15">
+        <v>65</v>
+      </c>
+      <c r="E15">
+        <v>70</v>
+      </c>
+      <c r="F15">
+        <v>55</v>
+      </c>
+      <c r="G15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>135</v>
+      </c>
+      <c r="D16">
+        <v>130</v>
+      </c>
+      <c r="E16">
+        <v>115</v>
+      </c>
+      <c r="F16">
+        <v>85</v>
+      </c>
+      <c r="G16">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>85</v>
+      </c>
+      <c r="D17">
+        <v>90</v>
+      </c>
+      <c r="E17">
+        <v>110</v>
+      </c>
+      <c r="F17">
+        <v>70</v>
+      </c>
+      <c r="G17">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>135</v>
+      </c>
+      <c r="D18">
+        <v>130</v>
+      </c>
+      <c r="E18">
+        <v>125</v>
+      </c>
+      <c r="F18">
+        <v>130</v>
+      </c>
+      <c r="G18">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>145</v>
+      </c>
+      <c r="D19">
+        <v>100</v>
+      </c>
+      <c r="E19">
+        <v>155</v>
+      </c>
+      <c r="F19">
+        <v>105</v>
+      </c>
+      <c r="G19">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>150</v>
+      </c>
+      <c r="D20">
+        <v>100</v>
+      </c>
+      <c r="E20">
+        <v>105</v>
+      </c>
+      <c r="F20">
+        <v>115</v>
+      </c>
+      <c r="G20">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>90</v>
+      </c>
+      <c r="D21">
+        <v>160</v>
+      </c>
+      <c r="E21">
+        <v>115</v>
+      </c>
+      <c r="F21">
+        <v>115</v>
+      </c>
+      <c r="G21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>100</v>
+      </c>
+      <c r="D22">
+        <v>140</v>
+      </c>
+      <c r="E22">
+        <v>110</v>
+      </c>
+      <c r="F22">
+        <v>95</v>
+      </c>
+      <c r="G22">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>85</v>
+      </c>
+      <c r="D23">
+        <v>75</v>
+      </c>
+      <c r="E23">
+        <v>75</v>
+      </c>
+      <c r="F23">
+        <v>50</v>
+      </c>
+      <c r="G23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>90</v>
+      </c>
+      <c r="D24">
+        <v>85</v>
+      </c>
+      <c r="E24">
+        <v>75</v>
+      </c>
+      <c r="F24">
+        <v>105</v>
+      </c>
+      <c r="G24">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>155</v>
+      </c>
+      <c r="D25">
+        <v>180</v>
+      </c>
+      <c r="E25">
+        <v>120</v>
+      </c>
+      <c r="F25">
+        <v>90</v>
+      </c>
+      <c r="G25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>175</v>
+      </c>
+      <c r="E26">
+        <v>155</v>
+      </c>
+      <c r="F26">
+        <v>130</v>
+      </c>
+      <c r="G26">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>130</v>
+      </c>
+      <c r="D27">
+        <v>55</v>
+      </c>
+      <c r="E27">
+        <v>105</v>
+      </c>
+      <c r="F27">
+        <v>130</v>
+      </c>
+      <c r="G27">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>125</v>
+      </c>
+      <c r="D28">
+        <v>90</v>
+      </c>
+      <c r="E28">
+        <v>100</v>
+      </c>
+      <c r="F28">
+        <v>105</v>
+      </c>
+      <c r="G28">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>185</v>
+      </c>
+      <c r="D29">
+        <v>160</v>
+      </c>
+      <c r="E29">
+        <v>160</v>
+      </c>
+      <c r="F29">
+        <v>130</v>
+      </c>
+      <c r="G29">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>80</v>
+      </c>
+      <c r="D30">
+        <v>85</v>
+      </c>
+      <c r="E30">
+        <v>95</v>
+      </c>
+      <c r="F30">
+        <v>95</v>
+      </c>
+      <c r="G30">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>130</v>
+      </c>
+      <c r="D31">
+        <v>120</v>
+      </c>
+      <c r="E31">
+        <v>120</v>
+      </c>
+      <c r="F31">
+        <v>120</v>
+      </c>
+      <c r="G31">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>125</v>
+      </c>
+      <c r="D32">
+        <v>95</v>
+      </c>
+      <c r="E32">
+        <v>80</v>
+      </c>
+      <c r="F32">
+        <v>80</v>
+      </c>
+      <c r="G32">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>120</v>
+      </c>
+      <c r="D33">
+        <v>145</v>
+      </c>
+      <c r="E33">
+        <v>105</v>
+      </c>
+      <c r="F33">
+        <v>130</v>
+      </c>
+      <c r="G33">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>120</v>
+      </c>
+      <c r="D34">
+        <v>120</v>
+      </c>
+      <c r="E34">
+        <v>140</v>
+      </c>
+      <c r="F34">
+        <v>140</v>
+      </c>
+      <c r="G34">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>90</v>
+      </c>
+      <c r="D35">
+        <v>90</v>
+      </c>
+      <c r="E35">
+        <v>80</v>
+      </c>
+      <c r="F35">
+        <v>120</v>
+      </c>
+      <c r="G35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>80</v>
+      </c>
+      <c r="D36">
+        <v>105</v>
+      </c>
+      <c r="E36">
+        <v>185</v>
+      </c>
+      <c r="F36">
+        <v>150</v>
+      </c>
+      <c r="G36">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>170</v>
+      </c>
+      <c r="D37">
+        <v>155</v>
+      </c>
+      <c r="E37">
+        <v>130</v>
+      </c>
+      <c r="F37">
+        <v>135</v>
+      </c>
+      <c r="G37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>155</v>
+      </c>
+      <c r="D38">
+        <v>70</v>
+      </c>
+      <c r="E38">
+        <v>60</v>
+      </c>
+      <c r="F38">
+        <v>50</v>
+      </c>
+      <c r="G38">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>100</v>
+      </c>
+      <c r="D39">
+        <v>135</v>
+      </c>
+      <c r="E39">
+        <v>95</v>
+      </c>
+      <c r="F39">
+        <v>100</v>
+      </c>
+      <c r="G39">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>115</v>
+      </c>
+      <c r="D40">
+        <v>130</v>
+      </c>
+      <c r="E40">
+        <v>125</v>
+      </c>
+      <c r="F40">
+        <v>105</v>
+      </c>
+      <c r="G40">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>120</v>
+      </c>
+      <c r="D41">
+        <v>60</v>
+      </c>
+      <c r="E41">
+        <v>110</v>
+      </c>
+      <c r="F41">
+        <v>75</v>
+      </c>
+      <c r="G41">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>125</v>
+      </c>
+      <c r="D42">
+        <v>110</v>
+      </c>
+      <c r="E42">
+        <v>110</v>
+      </c>
+      <c r="F42">
+        <v>120</v>
+      </c>
+      <c r="G42">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>125</v>
+      </c>
+      <c r="D43">
+        <v>150</v>
+      </c>
+      <c r="E43">
+        <v>130</v>
+      </c>
+      <c r="F43">
+        <v>150</v>
+      </c>
+      <c r="G43">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>75</v>
+      </c>
+      <c r="D44">
+        <v>85</v>
+      </c>
+      <c r="E44">
+        <v>85</v>
+      </c>
+      <c r="F44">
+        <v>90</v>
+      </c>
+      <c r="G44">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>145</v>
+      </c>
+      <c r="D45">
+        <v>90</v>
+      </c>
+      <c r="E45">
+        <v>60</v>
+      </c>
+      <c r="F45">
+        <v>105</v>
+      </c>
+      <c r="G45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>140</v>
+      </c>
+      <c r="D46">
+        <v>105</v>
+      </c>
+      <c r="E46">
+        <v>150</v>
+      </c>
+      <c r="F46">
+        <v>105</v>
+      </c>
+      <c r="G46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>150</v>
+      </c>
+      <c r="D47">
+        <v>155</v>
+      </c>
+      <c r="E47">
+        <v>165</v>
+      </c>
+      <c r="F47">
+        <v>140</v>
+      </c>
+      <c r="G47">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>140</v>
+      </c>
+      <c r="D48">
+        <v>140</v>
+      </c>
+      <c r="E48">
+        <v>135</v>
+      </c>
+      <c r="F48">
+        <v>80</v>
+      </c>
+      <c r="G48">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>95</v>
+      </c>
+      <c r="D49">
+        <v>95</v>
+      </c>
+      <c r="E49">
+        <v>115</v>
+      </c>
+      <c r="F49">
+        <v>65</v>
+      </c>
+      <c r="G49">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>110</v>
+      </c>
+      <c r="D50">
+        <v>85</v>
+      </c>
+      <c r="E50">
+        <v>135</v>
+      </c>
+      <c r="F50">
+        <v>110</v>
+      </c>
+      <c r="G50">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>115</v>
+      </c>
+      <c r="D51">
+        <v>95</v>
+      </c>
+      <c r="E51">
+        <v>140</v>
+      </c>
+      <c r="F51">
+        <v>95</v>
+      </c>
+      <c r="G51">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>95</v>
+      </c>
+      <c r="D52">
+        <v>95</v>
+      </c>
+      <c r="E52">
+        <v>50</v>
+      </c>
+      <c r="F52">
+        <v>110</v>
+      </c>
+      <c r="G52">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>85</v>
+      </c>
+      <c r="D53">
+        <v>125</v>
+      </c>
+      <c r="E53">
+        <v>145</v>
+      </c>
+      <c r="F53">
+        <v>110</v>
+      </c>
+      <c r="G53">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>145</v>
+      </c>
+      <c r="D54">
+        <v>130</v>
+      </c>
+      <c r="E54">
+        <v>100</v>
+      </c>
+      <c r="F54">
+        <v>95</v>
+      </c>
+      <c r="G54">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>50</v>
+      </c>
+      <c r="D55">
+        <v>85</v>
+      </c>
+      <c r="E55">
+        <v>80</v>
+      </c>
+      <c r="F55">
+        <v>70</v>
+      </c>
+      <c r="G55">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>85</v>
+      </c>
+      <c r="D56">
+        <v>85</v>
+      </c>
+      <c r="E56">
+        <v>115</v>
+      </c>
+      <c r="F56">
+        <v>105</v>
+      </c>
+      <c r="G56">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>135</v>
+      </c>
+      <c r="D57">
+        <v>80</v>
+      </c>
+      <c r="E57">
+        <v>75</v>
+      </c>
+      <c r="F57">
+        <v>130</v>
+      </c>
+      <c r="G57">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>95</v>
+      </c>
+      <c r="D58">
+        <v>140</v>
+      </c>
+      <c r="E58">
+        <v>125</v>
+      </c>
+      <c r="F58">
+        <v>110</v>
+      </c>
+      <c r="G58">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>100</v>
+      </c>
+      <c r="D59">
+        <v>110</v>
+      </c>
+      <c r="E59">
+        <v>100</v>
+      </c>
+      <c r="F59">
+        <v>80</v>
+      </c>
+      <c r="G59">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>140</v>
+      </c>
+      <c r="D60">
+        <v>100</v>
+      </c>
+      <c r="E60">
+        <v>105</v>
+      </c>
+      <c r="F60">
+        <v>85</v>
+      </c>
+      <c r="G60">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>115</v>
+      </c>
+      <c r="D61">
+        <v>120</v>
+      </c>
+      <c r="E61">
+        <v>115</v>
+      </c>
+      <c r="F61">
+        <v>125</v>
+      </c>
+      <c r="G61">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>95</v>
+      </c>
+      <c r="D62">
+        <v>90</v>
+      </c>
+      <c r="E62">
+        <v>100</v>
+      </c>
+      <c r="F62">
+        <v>135</v>
+      </c>
+      <c r="G62">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>145</v>
+      </c>
+      <c r="D63">
+        <v>135</v>
+      </c>
+      <c r="E63">
+        <v>125</v>
+      </c>
+      <c r="F63">
+        <v>120</v>
+      </c>
+      <c r="G63">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC17B69C-7AF4-4420-9BB3-BA81BA0BD0AA}">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" customWidth="1"/>
-    <col min="7" max="7" width="20.08984375" customWidth="1"/>
-    <col min="8" max="8" width="13.453125" customWidth="1"/>
-    <col min="9" max="9" width="7.08984375" customWidth="1"/>
-    <col min="10" max="10" width="12.90625" customWidth="1"/>
-    <col min="11" max="11" width="13.26953125" customWidth="1"/>
-    <col min="12" max="12" width="12.90625" customWidth="1"/>
-    <col min="13" max="13" width="13.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="16" max="16" width="16.7265625" customWidth="1"/>
+    <col min="16" max="16" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>79</v>
       </c>
@@ -3747,7 +5229,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -3776,7 +5258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3808,7 +5290,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3843,7 +5325,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3879,7 +5361,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3915,7 +5397,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3951,7 +5433,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3987,7 +5469,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -4022,7 +5504,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>52</v>
       </c>
@@ -4051,7 +5533,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>33</v>
       </c>
@@ -4080,7 +5562,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>70</v>
       </c>
@@ -4109,7 +5591,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>56</v>
       </c>
@@ -4138,7 +5620,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>36</v>
       </c>
@@ -4167,7 +5649,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>49</v>
       </c>
@@ -4196,7 +5678,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>60</v>
       </c>
@@ -4225,7 +5707,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>63</v>
       </c>
@@ -4254,7 +5736,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>47</v>
       </c>
@@ -4283,7 +5765,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>48</v>
       </c>
@@ -4312,7 +5794,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>69</v>
       </c>
@@ -4341,7 +5823,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>18</v>
       </c>
@@ -4370,7 +5852,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>55</v>
       </c>
@@ -4399,7 +5881,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>67</v>
       </c>
@@ -4428,7 +5910,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>35</v>
       </c>
@@ -4457,7 +5939,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>34</v>
       </c>
@@ -4486,7 +5968,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>15</v>
       </c>
@@ -4515,7 +5997,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>46</v>
       </c>
@@ -4544,7 +6026,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>24</v>
       </c>
@@ -4573,7 +6055,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>27</v>
       </c>
@@ -4602,7 +6084,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>8</v>
       </c>
@@ -4631,7 +6113,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>54</v>
       </c>
@@ -4660,7 +6142,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>37</v>
       </c>
@@ -4689,7 +6171,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>14</v>
       </c>
@@ -4718,7 +6200,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
         <v>31</v>
       </c>
@@ -4747,7 +6229,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
         <v>30</v>
       </c>
@@ -4776,7 +6258,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>32</v>
       </c>
@@ -4805,7 +6287,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
         <v>73</v>
       </c>
@@ -4834,7 +6316,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
         <v>41</v>
       </c>
@@ -4863,7 +6345,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>65</v>
       </c>
@@ -4892,7 +6374,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
         <v>68</v>
       </c>
@@ -4921,7 +6403,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
         <v>64</v>
       </c>
@@ -4950,7 +6432,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>58</v>
       </c>
@@ -4979,7 +6461,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
         <v>20</v>
       </c>
@@ -5008,7 +6490,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>62</v>
       </c>
@@ -5037,7 +6519,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
         <v>74</v>
       </c>
@@ -5066,7 +6548,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
         <v>29</v>
       </c>
@@ -5095,7 +6577,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
         <v>23</v>
       </c>
@@ -5124,7 +6606,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
         <v>40</v>
       </c>
@@ -5153,7 +6635,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="49" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
         <v>21</v>
       </c>
@@ -5182,7 +6664,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
         <v>44</v>
       </c>
@@ -5211,7 +6693,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
         <v>71</v>
       </c>
@@ -5240,7 +6722,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
         <v>57</v>
       </c>
@@ -5269,7 +6751,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
         <v>28</v>
       </c>
@@ -5298,7 +6780,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
         <v>53</v>
       </c>
@@ -5327,7 +6809,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
         <v>50</v>
       </c>
@@ -5356,7 +6838,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
         <v>75</v>
       </c>
@@ -5385,7 +6867,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
         <v>42</v>
       </c>
@@ -5414,7 +6896,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="58" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
         <v>45</v>
       </c>
@@ -5443,7 +6925,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
         <v>38</v>
       </c>
@@ -5472,7 +6954,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D60" t="s">
         <v>16</v>
       </c>
@@ -5501,7 +6983,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
         <v>59</v>
       </c>
@@ -5530,7 +7012,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
         <v>22</v>
       </c>
@@ -5559,7 +7041,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
         <v>39</v>
       </c>
@@ -5588,7 +7070,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
         <v>11</v>
       </c>
@@ -5625,7 +7107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B297E5BD-D2C2-4A6A-850B-6B3CD2ABF22D}">
   <dimension ref="B1:F161"/>
   <sheetViews>
@@ -5633,9 +7115,9 @@
       <selection activeCell="H162" sqref="H162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>76</v>
       </c>
@@ -5643,7 +7125,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>0</v>
       </c>
@@ -5657,7 +7139,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -5671,7 +7153,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0</v>
       </c>
@@ -5685,7 +7167,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>0</v>
       </c>
@@ -5699,7 +7181,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0</v>
       </c>
@@ -5713,7 +7195,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>0</v>
       </c>
@@ -5727,7 +7209,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>0</v>
       </c>
@@ -5741,7 +7223,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>0</v>
       </c>
@@ -5755,7 +7237,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>0</v>
       </c>
@@ -5769,7 +7251,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>0</v>
       </c>
@@ -5783,7 +7265,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>0</v>
       </c>
@@ -5797,7 +7279,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>0</v>
       </c>
@@ -5811,7 +7293,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>0</v>
       </c>
@@ -5825,7 +7307,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>0</v>
       </c>
@@ -5839,7 +7321,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>0</v>
       </c>
@@ -5853,7 +7335,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>0</v>
       </c>
@@ -5867,7 +7349,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>0</v>
       </c>
@@ -5881,7 +7363,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>0</v>
       </c>
@@ -5895,7 +7377,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>0</v>
       </c>
@@ -5909,7 +7391,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>0</v>
       </c>
@@ -5923,7 +7405,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>0</v>
       </c>
@@ -5937,7 +7419,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>0</v>
       </c>
@@ -5951,7 +7433,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>0</v>
       </c>
@@ -5965,7 +7447,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>0</v>
       </c>
@@ -5979,7 +7461,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>0</v>
       </c>
@@ -5993,7 +7475,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>0</v>
       </c>
@@ -6007,7 +7489,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>0</v>
       </c>
@@ -6021,7 +7503,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>0</v>
       </c>
@@ -6035,7 +7517,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>0</v>
       </c>
@@ -6049,7 +7531,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>0</v>
       </c>
@@ -6063,7 +7545,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>0</v>
       </c>
@@ -6077,7 +7559,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>0</v>
       </c>
@@ -6091,7 +7573,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>1</v>
       </c>
@@ -6105,7 +7587,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>1</v>
       </c>
@@ -6119,7 +7601,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>1</v>
       </c>
@@ -6133,7 +7615,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>1</v>
       </c>
@@ -6147,7 +7629,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>1</v>
       </c>
@@ -6161,7 +7643,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>1</v>
       </c>
@@ -6175,7 +7657,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>1</v>
       </c>
@@ -6189,7 +7671,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>1</v>
       </c>
@@ -6203,7 +7685,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>1</v>
       </c>
@@ -6217,7 +7699,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>1</v>
       </c>
@@ -6231,7 +7713,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44">
         <v>1</v>
       </c>
@@ -6245,7 +7727,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>1</v>
       </c>
@@ -6259,7 +7741,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>1</v>
       </c>
@@ -6273,7 +7755,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>1</v>
       </c>
@@ -6287,7 +7769,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>1</v>
       </c>
@@ -6301,7 +7783,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>1</v>
       </c>
@@ -6315,7 +7797,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>1</v>
       </c>
@@ -6329,7 +7811,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>1</v>
       </c>
@@ -6343,7 +7825,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>1</v>
       </c>
@@ -6357,7 +7839,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53">
         <v>1</v>
       </c>
@@ -6371,7 +7853,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>1</v>
       </c>
@@ -6385,7 +7867,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>1</v>
       </c>
@@ -6399,7 +7881,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>1</v>
       </c>
@@ -6413,7 +7895,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57">
         <v>1</v>
       </c>
@@ -6427,7 +7909,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>1</v>
       </c>
@@ -6441,7 +7923,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59">
         <v>1</v>
       </c>
@@ -6455,7 +7937,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60">
         <v>1</v>
       </c>
@@ -6469,7 +7951,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61">
         <v>1</v>
       </c>
@@ -6483,7 +7965,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62">
         <v>1</v>
       </c>
@@ -6497,7 +7979,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63">
         <v>1</v>
       </c>
@@ -6511,7 +7993,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64">
         <v>1</v>
       </c>
@@ -6525,7 +8007,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65">
         <v>1</v>
       </c>
@@ -6539,7 +8021,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66">
         <v>2</v>
       </c>
@@ -6553,7 +8035,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67">
         <v>2</v>
       </c>
@@ -6567,7 +8049,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68">
         <v>2</v>
       </c>
@@ -6581,7 +8063,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69">
         <v>2</v>
       </c>
@@ -6595,7 +8077,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70">
         <v>2</v>
       </c>
@@ -6609,7 +8091,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71">
         <v>2</v>
       </c>
@@ -6623,7 +8105,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72">
         <v>2</v>
       </c>
@@ -6637,7 +8119,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73">
         <v>2</v>
       </c>
@@ -6651,7 +8133,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74">
         <v>2</v>
       </c>
@@ -6665,7 +8147,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75">
         <v>2</v>
       </c>
@@ -6679,7 +8161,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B76">
         <v>2</v>
       </c>
@@ -6693,7 +8175,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77">
         <v>2</v>
       </c>
@@ -6707,7 +8189,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78">
         <v>2</v>
       </c>
@@ -6721,7 +8203,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79">
         <v>2</v>
       </c>
@@ -6735,7 +8217,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80">
         <v>2</v>
       </c>
@@ -6749,7 +8231,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B81">
         <v>2</v>
       </c>
@@ -6763,7 +8245,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B82">
         <v>2</v>
       </c>
@@ -6777,7 +8259,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B83">
         <v>2</v>
       </c>
@@ -6791,7 +8273,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B84">
         <v>2</v>
       </c>
@@ -6805,7 +8287,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85">
         <v>2</v>
       </c>
@@ -6819,7 +8301,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B86">
         <v>2</v>
       </c>
@@ -6833,7 +8315,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B87">
         <v>2</v>
       </c>
@@ -6847,7 +8329,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B88">
         <v>2</v>
       </c>
@@ -6861,7 +8343,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B89">
         <v>2</v>
       </c>
@@ -6875,7 +8357,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B90">
         <v>2</v>
       </c>
@@ -6889,7 +8371,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B91">
         <v>2</v>
       </c>
@@ -6903,7 +8385,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B92">
         <v>2</v>
       </c>
@@ -6917,7 +8399,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B93">
         <v>2</v>
       </c>
@@ -6931,7 +8413,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B94">
         <v>2</v>
       </c>
@@ -6945,7 +8427,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B95">
         <v>2</v>
       </c>
@@ -6959,7 +8441,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B96">
         <v>2</v>
       </c>
@@ -6973,7 +8455,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B97">
         <v>2</v>
       </c>
@@ -6987,7 +8469,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B98">
         <v>3</v>
       </c>
@@ -7001,7 +8483,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B99">
         <v>3</v>
       </c>
@@ -7015,7 +8497,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B100">
         <v>3</v>
       </c>
@@ -7029,7 +8511,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101">
         <v>3</v>
       </c>
@@ -7043,7 +8525,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102">
         <v>3</v>
       </c>
@@ -7057,7 +8539,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103">
         <v>3</v>
       </c>
@@ -7071,7 +8553,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B104">
         <v>3</v>
       </c>
@@ -7085,7 +8567,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B105">
         <v>3</v>
       </c>
@@ -7099,7 +8581,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106">
         <v>3</v>
       </c>
@@ -7113,7 +8595,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107">
         <v>3</v>
       </c>
@@ -7127,7 +8609,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B108">
         <v>3</v>
       </c>
@@ -7141,7 +8623,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B109">
         <v>3</v>
       </c>
@@ -7155,7 +8637,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B110">
         <v>3</v>
       </c>
@@ -7169,7 +8651,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B111">
         <v>3</v>
       </c>
@@ -7183,7 +8665,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B112">
         <v>3</v>
       </c>
@@ -7197,7 +8679,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B113">
         <v>3</v>
       </c>
@@ -7211,7 +8693,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B114">
         <v>3</v>
       </c>
@@ -7225,7 +8707,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B115">
         <v>3</v>
       </c>
@@ -7239,7 +8721,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B116">
         <v>3</v>
       </c>
@@ -7253,7 +8735,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B117">
         <v>3</v>
       </c>
@@ -7267,7 +8749,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B118">
         <v>3</v>
       </c>
@@ -7281,7 +8763,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B119">
         <v>3</v>
       </c>
@@ -7295,7 +8777,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B120">
         <v>3</v>
       </c>
@@ -7309,7 +8791,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B121">
         <v>3</v>
       </c>
@@ -7323,7 +8805,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B122">
         <v>3</v>
       </c>
@@ -7337,7 +8819,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B123">
         <v>3</v>
       </c>
@@ -7351,7 +8833,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B124">
         <v>3</v>
       </c>
@@ -7365,7 +8847,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B125">
         <v>3</v>
       </c>
@@ -7379,7 +8861,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B126">
         <v>3</v>
       </c>
@@ -7393,7 +8875,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B127">
         <v>3</v>
       </c>
@@ -7407,7 +8889,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B128">
         <v>3</v>
       </c>
@@ -7421,7 +8903,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129">
         <v>3</v>
       </c>
@@ -7435,7 +8917,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130">
         <v>4</v>
       </c>
@@ -7449,7 +8931,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B131">
         <v>4</v>
       </c>
@@ -7463,7 +8945,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B132">
         <v>4</v>
       </c>
@@ -7477,7 +8959,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B133">
         <v>4</v>
       </c>
@@ -7491,7 +8973,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B134">
         <v>4</v>
       </c>
@@ -7505,7 +8987,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B135">
         <v>4</v>
       </c>
@@ -7519,7 +9001,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B136">
         <v>4</v>
       </c>
@@ -7533,7 +9015,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B137">
         <v>4</v>
       </c>
@@ -7547,7 +9029,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B138">
         <v>4</v>
       </c>
@@ -7561,7 +9043,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B139">
         <v>4</v>
       </c>
@@ -7575,7 +9057,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B140">
         <v>4</v>
       </c>
@@ -7589,7 +9071,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B141">
         <v>4</v>
       </c>
@@ -7603,7 +9085,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B142">
         <v>4</v>
       </c>
@@ -7617,7 +9099,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B143">
         <v>4</v>
       </c>
@@ -7631,7 +9113,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B144">
         <v>4</v>
       </c>
@@ -7645,7 +9127,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B145">
         <v>4</v>
       </c>
@@ -7659,7 +9141,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B146">
         <v>4</v>
       </c>
@@ -7673,7 +9155,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B147">
         <v>4</v>
       </c>
@@ -7687,7 +9169,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B148">
         <v>4</v>
       </c>
@@ -7701,7 +9183,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B149">
         <v>4</v>
       </c>
@@ -7715,7 +9197,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B150">
         <v>4</v>
       </c>
@@ -7729,7 +9211,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B151">
         <v>4</v>
       </c>
@@ -7743,7 +9225,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B152">
         <v>4</v>
       </c>
@@ -7751,7 +9233,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B153">
         <v>4</v>
       </c>
@@ -7759,7 +9241,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B154">
         <v>4</v>
       </c>
@@ -7767,7 +9249,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B155">
         <v>4</v>
       </c>
@@ -7775,7 +9257,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B156">
         <v>4</v>
       </c>
@@ -7783,7 +9265,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B157">
         <v>4</v>
       </c>
@@ -7791,7 +9273,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B158">
         <v>4</v>
       </c>
@@ -7799,7 +9281,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B159">
         <v>4</v>
       </c>
@@ -7807,7 +9289,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B160">
         <v>4</v>
       </c>
@@ -7815,7 +9297,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B161">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
fitted linear models to both control and valerian data sets
</commit_message>
<xml_diff>
--- a/Research Project Data File.xlsx
+++ b/Research Project Data File.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ec892e7e4853af95/Documents/UNI/UNI 1 SEM 2/STAT1301/Research/Arthur-s-STAT1301-Project-on-Valerian-Root/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="528" documentId="8_{9311CA3D-7FF6-4128-B46A-1A9324E1D225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{932F8BC7-AE1F-4CD6-925E-38BF3873E2AA}"/>
+  <xr:revisionPtr revIDLastSave="557" documentId="8_{9311CA3D-7FF6-4128-B46A-1A9324E1D225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CE0E2E5-0BB6-47FF-8ECB-3CE06C7E3C64}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B1D913C5-7F24-403E-865C-599D1658A181}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B1D913C5-7F24-403E-865C-599D1658A181}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3402,6 +3402,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3718,1490 +3722,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB63271F-69B0-4854-9623-6BAC9B90FB1F}">
-  <dimension ref="A1:G63"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" customWidth="1"/>
-    <col min="9" max="9" width="7.109375" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.21875" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" customWidth="1"/>
-    <col min="13" max="13" width="13.21875" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="16" max="16" width="16.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>4</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>90</v>
-      </c>
-      <c r="D2">
-        <v>120</v>
-      </c>
-      <c r="E2">
-        <v>105</v>
-      </c>
-      <c r="F2">
-        <v>175</v>
-      </c>
-      <c r="G2">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>110</v>
-      </c>
-      <c r="D3">
-        <v>110</v>
-      </c>
-      <c r="E3">
-        <v>95</v>
-      </c>
-      <c r="F3">
-        <v>130</v>
-      </c>
-      <c r="G3">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>155</v>
-      </c>
-      <c r="D4">
-        <v>170</v>
-      </c>
-      <c r="E4">
-        <v>145</v>
-      </c>
-      <c r="F4">
-        <v>155</v>
-      </c>
-      <c r="G4">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>150</v>
-      </c>
-      <c r="D5">
-        <v>155</v>
-      </c>
-      <c r="E5">
-        <v>105</v>
-      </c>
-      <c r="F5">
-        <v>90</v>
-      </c>
-      <c r="G5">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>120</v>
-      </c>
-      <c r="D6">
-        <v>125</v>
-      </c>
-      <c r="E6">
-        <v>55</v>
-      </c>
-      <c r="F6">
-        <v>55</v>
-      </c>
-      <c r="G6">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>75</v>
-      </c>
-      <c r="D7">
-        <v>110</v>
-      </c>
-      <c r="E7">
-        <v>120</v>
-      </c>
-      <c r="F7">
-        <v>85</v>
-      </c>
-      <c r="G7">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>90</v>
-      </c>
-      <c r="D8">
-        <v>85</v>
-      </c>
-      <c r="E8">
-        <v>65</v>
-      </c>
-      <c r="F8">
-        <v>75</v>
-      </c>
-      <c r="G8">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>140</v>
-      </c>
-      <c r="D9">
-        <v>120</v>
-      </c>
-      <c r="E9">
-        <v>100</v>
-      </c>
-      <c r="F9">
-        <v>110</v>
-      </c>
-      <c r="G9">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>175</v>
-      </c>
-      <c r="D10">
-        <v>140</v>
-      </c>
-      <c r="E10">
-        <v>160</v>
-      </c>
-      <c r="F10">
-        <v>155</v>
-      </c>
-      <c r="G10">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>120</v>
-      </c>
-      <c r="D11">
-        <v>85</v>
-      </c>
-      <c r="E11">
-        <v>130</v>
-      </c>
-      <c r="F11">
-        <v>115</v>
-      </c>
-      <c r="G11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>150</v>
-      </c>
-      <c r="D12">
-        <v>180</v>
-      </c>
-      <c r="E12">
-        <v>130</v>
-      </c>
-      <c r="F12">
-        <v>165</v>
-      </c>
-      <c r="G12">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>170</v>
-      </c>
-      <c r="D13">
-        <v>155</v>
-      </c>
-      <c r="E13">
-        <v>110</v>
-      </c>
-      <c r="F13">
-        <v>135</v>
-      </c>
-      <c r="G13">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>150</v>
-      </c>
-      <c r="D14">
-        <v>110</v>
-      </c>
-      <c r="E14">
-        <v>125</v>
-      </c>
-      <c r="F14">
-        <v>100</v>
-      </c>
-      <c r="G14">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>75</v>
-      </c>
-      <c r="D15">
-        <v>65</v>
-      </c>
-      <c r="E15">
-        <v>70</v>
-      </c>
-      <c r="F15">
-        <v>55</v>
-      </c>
-      <c r="G15">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>135</v>
-      </c>
-      <c r="D16">
-        <v>130</v>
-      </c>
-      <c r="E16">
-        <v>115</v>
-      </c>
-      <c r="F16">
-        <v>85</v>
-      </c>
-      <c r="G16">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>85</v>
-      </c>
-      <c r="D17">
-        <v>90</v>
-      </c>
-      <c r="E17">
-        <v>110</v>
-      </c>
-      <c r="F17">
-        <v>70</v>
-      </c>
-      <c r="G17">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>135</v>
-      </c>
-      <c r="D18">
-        <v>130</v>
-      </c>
-      <c r="E18">
-        <v>125</v>
-      </c>
-      <c r="F18">
-        <v>130</v>
-      </c>
-      <c r="G18">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>145</v>
-      </c>
-      <c r="D19">
-        <v>100</v>
-      </c>
-      <c r="E19">
-        <v>155</v>
-      </c>
-      <c r="F19">
-        <v>105</v>
-      </c>
-      <c r="G19">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>150</v>
-      </c>
-      <c r="D20">
-        <v>100</v>
-      </c>
-      <c r="E20">
-        <v>105</v>
-      </c>
-      <c r="F20">
-        <v>115</v>
-      </c>
-      <c r="G20">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>90</v>
-      </c>
-      <c r="D21">
-        <v>160</v>
-      </c>
-      <c r="E21">
-        <v>115</v>
-      </c>
-      <c r="F21">
-        <v>115</v>
-      </c>
-      <c r="G21">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>100</v>
-      </c>
-      <c r="D22">
-        <v>140</v>
-      </c>
-      <c r="E22">
-        <v>110</v>
-      </c>
-      <c r="F22">
-        <v>95</v>
-      </c>
-      <c r="G22">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>85</v>
-      </c>
-      <c r="D23">
-        <v>75</v>
-      </c>
-      <c r="E23">
-        <v>75</v>
-      </c>
-      <c r="F23">
-        <v>50</v>
-      </c>
-      <c r="G23">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>90</v>
-      </c>
-      <c r="D24">
-        <v>85</v>
-      </c>
-      <c r="E24">
-        <v>75</v>
-      </c>
-      <c r="F24">
-        <v>105</v>
-      </c>
-      <c r="G24">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>155</v>
-      </c>
-      <c r="D25">
-        <v>180</v>
-      </c>
-      <c r="E25">
-        <v>120</v>
-      </c>
-      <c r="F25">
-        <v>90</v>
-      </c>
-      <c r="G25">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>100</v>
-      </c>
-      <c r="D26">
-        <v>175</v>
-      </c>
-      <c r="E26">
-        <v>155</v>
-      </c>
-      <c r="F26">
-        <v>130</v>
-      </c>
-      <c r="G26">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>130</v>
-      </c>
-      <c r="D27">
-        <v>55</v>
-      </c>
-      <c r="E27">
-        <v>105</v>
-      </c>
-      <c r="F27">
-        <v>130</v>
-      </c>
-      <c r="G27">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>125</v>
-      </c>
-      <c r="D28">
-        <v>90</v>
-      </c>
-      <c r="E28">
-        <v>100</v>
-      </c>
-      <c r="F28">
-        <v>105</v>
-      </c>
-      <c r="G28">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>185</v>
-      </c>
-      <c r="D29">
-        <v>160</v>
-      </c>
-      <c r="E29">
-        <v>160</v>
-      </c>
-      <c r="F29">
-        <v>130</v>
-      </c>
-      <c r="G29">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>80</v>
-      </c>
-      <c r="D30">
-        <v>85</v>
-      </c>
-      <c r="E30">
-        <v>95</v>
-      </c>
-      <c r="F30">
-        <v>95</v>
-      </c>
-      <c r="G30">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>130</v>
-      </c>
-      <c r="D31">
-        <v>120</v>
-      </c>
-      <c r="E31">
-        <v>120</v>
-      </c>
-      <c r="F31">
-        <v>120</v>
-      </c>
-      <c r="G31">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>125</v>
-      </c>
-      <c r="D32">
-        <v>95</v>
-      </c>
-      <c r="E32">
-        <v>80</v>
-      </c>
-      <c r="F32">
-        <v>80</v>
-      </c>
-      <c r="G32">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>120</v>
-      </c>
-      <c r="D33">
-        <v>145</v>
-      </c>
-      <c r="E33">
-        <v>105</v>
-      </c>
-      <c r="F33">
-        <v>130</v>
-      </c>
-      <c r="G33">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>120</v>
-      </c>
-      <c r="D34">
-        <v>120</v>
-      </c>
-      <c r="E34">
-        <v>140</v>
-      </c>
-      <c r="F34">
-        <v>140</v>
-      </c>
-      <c r="G34">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>90</v>
-      </c>
-      <c r="D35">
-        <v>90</v>
-      </c>
-      <c r="E35">
-        <v>80</v>
-      </c>
-      <c r="F35">
-        <v>120</v>
-      </c>
-      <c r="G35">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>80</v>
-      </c>
-      <c r="D36">
-        <v>105</v>
-      </c>
-      <c r="E36">
-        <v>185</v>
-      </c>
-      <c r="F36">
-        <v>150</v>
-      </c>
-      <c r="G36">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37">
-        <v>170</v>
-      </c>
-      <c r="D37">
-        <v>155</v>
-      </c>
-      <c r="E37">
-        <v>130</v>
-      </c>
-      <c r="F37">
-        <v>135</v>
-      </c>
-      <c r="G37">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>155</v>
-      </c>
-      <c r="D38">
-        <v>70</v>
-      </c>
-      <c r="E38">
-        <v>60</v>
-      </c>
-      <c r="F38">
-        <v>50</v>
-      </c>
-      <c r="G38">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>100</v>
-      </c>
-      <c r="D39">
-        <v>135</v>
-      </c>
-      <c r="E39">
-        <v>95</v>
-      </c>
-      <c r="F39">
-        <v>100</v>
-      </c>
-      <c r="G39">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>115</v>
-      </c>
-      <c r="D40">
-        <v>130</v>
-      </c>
-      <c r="E40">
-        <v>125</v>
-      </c>
-      <c r="F40">
-        <v>105</v>
-      </c>
-      <c r="G40">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>120</v>
-      </c>
-      <c r="D41">
-        <v>60</v>
-      </c>
-      <c r="E41">
-        <v>110</v>
-      </c>
-      <c r="F41">
-        <v>75</v>
-      </c>
-      <c r="G41">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>125</v>
-      </c>
-      <c r="D42">
-        <v>110</v>
-      </c>
-      <c r="E42">
-        <v>110</v>
-      </c>
-      <c r="F42">
-        <v>120</v>
-      </c>
-      <c r="G42">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>125</v>
-      </c>
-      <c r="D43">
-        <v>150</v>
-      </c>
-      <c r="E43">
-        <v>130</v>
-      </c>
-      <c r="F43">
-        <v>150</v>
-      </c>
-      <c r="G43">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>75</v>
-      </c>
-      <c r="D44">
-        <v>85</v>
-      </c>
-      <c r="E44">
-        <v>85</v>
-      </c>
-      <c r="F44">
-        <v>90</v>
-      </c>
-      <c r="G44">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>145</v>
-      </c>
-      <c r="D45">
-        <v>90</v>
-      </c>
-      <c r="E45">
-        <v>60</v>
-      </c>
-      <c r="F45">
-        <v>105</v>
-      </c>
-      <c r="G45">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46">
-        <v>140</v>
-      </c>
-      <c r="D46">
-        <v>105</v>
-      </c>
-      <c r="E46">
-        <v>150</v>
-      </c>
-      <c r="F46">
-        <v>105</v>
-      </c>
-      <c r="G46">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>150</v>
-      </c>
-      <c r="D47">
-        <v>155</v>
-      </c>
-      <c r="E47">
-        <v>165</v>
-      </c>
-      <c r="F47">
-        <v>140</v>
-      </c>
-      <c r="G47">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48">
-        <v>140</v>
-      </c>
-      <c r="D48">
-        <v>140</v>
-      </c>
-      <c r="E48">
-        <v>135</v>
-      </c>
-      <c r="F48">
-        <v>80</v>
-      </c>
-      <c r="G48">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <v>95</v>
-      </c>
-      <c r="D49">
-        <v>95</v>
-      </c>
-      <c r="E49">
-        <v>115</v>
-      </c>
-      <c r="F49">
-        <v>65</v>
-      </c>
-      <c r="G49">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>110</v>
-      </c>
-      <c r="D50">
-        <v>85</v>
-      </c>
-      <c r="E50">
-        <v>135</v>
-      </c>
-      <c r="F50">
-        <v>110</v>
-      </c>
-      <c r="G50">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51">
-        <v>115</v>
-      </c>
-      <c r="D51">
-        <v>95</v>
-      </c>
-      <c r="E51">
-        <v>140</v>
-      </c>
-      <c r="F51">
-        <v>95</v>
-      </c>
-      <c r="G51">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52">
-        <v>95</v>
-      </c>
-      <c r="D52">
-        <v>95</v>
-      </c>
-      <c r="E52">
-        <v>50</v>
-      </c>
-      <c r="F52">
-        <v>110</v>
-      </c>
-      <c r="G52">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53">
-        <v>85</v>
-      </c>
-      <c r="D53">
-        <v>125</v>
-      </c>
-      <c r="E53">
-        <v>145</v>
-      </c>
-      <c r="F53">
-        <v>110</v>
-      </c>
-      <c r="G53">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54">
-        <v>145</v>
-      </c>
-      <c r="D54">
-        <v>130</v>
-      </c>
-      <c r="E54">
-        <v>100</v>
-      </c>
-      <c r="F54">
-        <v>95</v>
-      </c>
-      <c r="G54">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55">
-        <v>50</v>
-      </c>
-      <c r="D55">
-        <v>85</v>
-      </c>
-      <c r="E55">
-        <v>80</v>
-      </c>
-      <c r="F55">
-        <v>70</v>
-      </c>
-      <c r="G55">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56">
-        <v>85</v>
-      </c>
-      <c r="D56">
-        <v>85</v>
-      </c>
-      <c r="E56">
-        <v>115</v>
-      </c>
-      <c r="F56">
-        <v>105</v>
-      </c>
-      <c r="G56">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57">
-        <v>135</v>
-      </c>
-      <c r="D57">
-        <v>80</v>
-      </c>
-      <c r="E57">
-        <v>75</v>
-      </c>
-      <c r="F57">
-        <v>130</v>
-      </c>
-      <c r="G57">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58">
-        <v>95</v>
-      </c>
-      <c r="D58">
-        <v>140</v>
-      </c>
-      <c r="E58">
-        <v>125</v>
-      </c>
-      <c r="F58">
-        <v>110</v>
-      </c>
-      <c r="G58">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59">
-        <v>100</v>
-      </c>
-      <c r="D59">
-        <v>110</v>
-      </c>
-      <c r="E59">
-        <v>100</v>
-      </c>
-      <c r="F59">
-        <v>80</v>
-      </c>
-      <c r="G59">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60">
-        <v>140</v>
-      </c>
-      <c r="D60">
-        <v>100</v>
-      </c>
-      <c r="E60">
-        <v>105</v>
-      </c>
-      <c r="F60">
-        <v>85</v>
-      </c>
-      <c r="G60">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-      <c r="C61">
-        <v>115</v>
-      </c>
-      <c r="D61">
-        <v>120</v>
-      </c>
-      <c r="E61">
-        <v>115</v>
-      </c>
-      <c r="F61">
-        <v>125</v>
-      </c>
-      <c r="G61">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-      <c r="C62">
-        <v>95</v>
-      </c>
-      <c r="D62">
-        <v>90</v>
-      </c>
-      <c r="E62">
-        <v>100</v>
-      </c>
-      <c r="F62">
-        <v>135</v>
-      </c>
-      <c r="G62">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-      <c r="C63">
-        <v>145</v>
-      </c>
-      <c r="D63">
-        <v>135</v>
-      </c>
-      <c r="E63">
-        <v>125</v>
-      </c>
-      <c r="F63">
-        <v>120</v>
-      </c>
-      <c r="G63">
-        <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC17B69C-7AF4-4420-9BB3-BA81BA0BD0AA}">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:L64"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7107,7 +5633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B297E5BD-D2C2-4A6A-850B-6B3CD2ABF22D}">
   <dimension ref="B1:F161"/>
   <sheetViews>
@@ -9309,4 +7835,1468 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51144233-ACDB-4F27-9520-ABAB64CF79CD}">
+  <dimension ref="A1:G63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>2</v>
+      </c>
+      <c r="F1">
+        <v>3</v>
+      </c>
+      <c r="G1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>90</v>
+      </c>
+      <c r="D2">
+        <v>120</v>
+      </c>
+      <c r="E2">
+        <v>105</v>
+      </c>
+      <c r="F2">
+        <v>175</v>
+      </c>
+      <c r="G2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>110</v>
+      </c>
+      <c r="D3">
+        <v>110</v>
+      </c>
+      <c r="E3">
+        <v>95</v>
+      </c>
+      <c r="F3">
+        <v>130</v>
+      </c>
+      <c r="G3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>155</v>
+      </c>
+      <c r="D4">
+        <v>170</v>
+      </c>
+      <c r="E4">
+        <v>145</v>
+      </c>
+      <c r="F4">
+        <v>155</v>
+      </c>
+      <c r="G4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>150</v>
+      </c>
+      <c r="D5">
+        <v>155</v>
+      </c>
+      <c r="E5">
+        <v>105</v>
+      </c>
+      <c r="F5">
+        <v>90</v>
+      </c>
+      <c r="G5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>120</v>
+      </c>
+      <c r="D6">
+        <v>125</v>
+      </c>
+      <c r="E6">
+        <v>55</v>
+      </c>
+      <c r="F6">
+        <v>55</v>
+      </c>
+      <c r="G6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>75</v>
+      </c>
+      <c r="D7">
+        <v>110</v>
+      </c>
+      <c r="E7">
+        <v>120</v>
+      </c>
+      <c r="F7">
+        <v>85</v>
+      </c>
+      <c r="G7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>90</v>
+      </c>
+      <c r="D8">
+        <v>85</v>
+      </c>
+      <c r="E8">
+        <v>65</v>
+      </c>
+      <c r="F8">
+        <v>75</v>
+      </c>
+      <c r="G8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>140</v>
+      </c>
+      <c r="D9">
+        <v>120</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>110</v>
+      </c>
+      <c r="G9">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>175</v>
+      </c>
+      <c r="D10">
+        <v>140</v>
+      </c>
+      <c r="E10">
+        <v>160</v>
+      </c>
+      <c r="F10">
+        <v>155</v>
+      </c>
+      <c r="G10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>120</v>
+      </c>
+      <c r="D11">
+        <v>85</v>
+      </c>
+      <c r="E11">
+        <v>130</v>
+      </c>
+      <c r="F11">
+        <v>115</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>150</v>
+      </c>
+      <c r="D12">
+        <v>180</v>
+      </c>
+      <c r="E12">
+        <v>130</v>
+      </c>
+      <c r="F12">
+        <v>165</v>
+      </c>
+      <c r="G12">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>170</v>
+      </c>
+      <c r="D13">
+        <v>155</v>
+      </c>
+      <c r="E13">
+        <v>110</v>
+      </c>
+      <c r="F13">
+        <v>135</v>
+      </c>
+      <c r="G13">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>150</v>
+      </c>
+      <c r="D14">
+        <v>110</v>
+      </c>
+      <c r="E14">
+        <v>125</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>75</v>
+      </c>
+      <c r="D15">
+        <v>65</v>
+      </c>
+      <c r="E15">
+        <v>70</v>
+      </c>
+      <c r="F15">
+        <v>55</v>
+      </c>
+      <c r="G15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>135</v>
+      </c>
+      <c r="D16">
+        <v>130</v>
+      </c>
+      <c r="E16">
+        <v>115</v>
+      </c>
+      <c r="F16">
+        <v>85</v>
+      </c>
+      <c r="G16">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>85</v>
+      </c>
+      <c r="D17">
+        <v>90</v>
+      </c>
+      <c r="E17">
+        <v>110</v>
+      </c>
+      <c r="F17">
+        <v>70</v>
+      </c>
+      <c r="G17">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>135</v>
+      </c>
+      <c r="D18">
+        <v>130</v>
+      </c>
+      <c r="E18">
+        <v>125</v>
+      </c>
+      <c r="F18">
+        <v>130</v>
+      </c>
+      <c r="G18">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>145</v>
+      </c>
+      <c r="D19">
+        <v>100</v>
+      </c>
+      <c r="E19">
+        <v>155</v>
+      </c>
+      <c r="F19">
+        <v>105</v>
+      </c>
+      <c r="G19">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>150</v>
+      </c>
+      <c r="D20">
+        <v>100</v>
+      </c>
+      <c r="E20">
+        <v>105</v>
+      </c>
+      <c r="F20">
+        <v>115</v>
+      </c>
+      <c r="G20">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>90</v>
+      </c>
+      <c r="D21">
+        <v>160</v>
+      </c>
+      <c r="E21">
+        <v>115</v>
+      </c>
+      <c r="F21">
+        <v>115</v>
+      </c>
+      <c r="G21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>100</v>
+      </c>
+      <c r="D22">
+        <v>140</v>
+      </c>
+      <c r="E22">
+        <v>110</v>
+      </c>
+      <c r="F22">
+        <v>95</v>
+      </c>
+      <c r="G22">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>85</v>
+      </c>
+      <c r="D23">
+        <v>75</v>
+      </c>
+      <c r="E23">
+        <v>75</v>
+      </c>
+      <c r="F23">
+        <v>50</v>
+      </c>
+      <c r="G23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>90</v>
+      </c>
+      <c r="D24">
+        <v>85</v>
+      </c>
+      <c r="E24">
+        <v>75</v>
+      </c>
+      <c r="F24">
+        <v>105</v>
+      </c>
+      <c r="G24">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>155</v>
+      </c>
+      <c r="D25">
+        <v>180</v>
+      </c>
+      <c r="E25">
+        <v>120</v>
+      </c>
+      <c r="F25">
+        <v>90</v>
+      </c>
+      <c r="G25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>175</v>
+      </c>
+      <c r="E26">
+        <v>155</v>
+      </c>
+      <c r="F26">
+        <v>130</v>
+      </c>
+      <c r="G26">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>130</v>
+      </c>
+      <c r="D27">
+        <v>55</v>
+      </c>
+      <c r="E27">
+        <v>105</v>
+      </c>
+      <c r="F27">
+        <v>130</v>
+      </c>
+      <c r="G27">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>125</v>
+      </c>
+      <c r="D28">
+        <v>90</v>
+      </c>
+      <c r="E28">
+        <v>100</v>
+      </c>
+      <c r="F28">
+        <v>105</v>
+      </c>
+      <c r="G28">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>185</v>
+      </c>
+      <c r="D29">
+        <v>160</v>
+      </c>
+      <c r="E29">
+        <v>160</v>
+      </c>
+      <c r="F29">
+        <v>130</v>
+      </c>
+      <c r="G29">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>80</v>
+      </c>
+      <c r="D30">
+        <v>85</v>
+      </c>
+      <c r="E30">
+        <v>95</v>
+      </c>
+      <c r="F30">
+        <v>95</v>
+      </c>
+      <c r="G30">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>130</v>
+      </c>
+      <c r="D31">
+        <v>120</v>
+      </c>
+      <c r="E31">
+        <v>120</v>
+      </c>
+      <c r="F31">
+        <v>120</v>
+      </c>
+      <c r="G31">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>125</v>
+      </c>
+      <c r="D32">
+        <v>95</v>
+      </c>
+      <c r="E32">
+        <v>80</v>
+      </c>
+      <c r="F32">
+        <v>80</v>
+      </c>
+      <c r="G32">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>120</v>
+      </c>
+      <c r="D33">
+        <v>145</v>
+      </c>
+      <c r="E33">
+        <v>105</v>
+      </c>
+      <c r="F33">
+        <v>130</v>
+      </c>
+      <c r="G33">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>120</v>
+      </c>
+      <c r="D34">
+        <v>120</v>
+      </c>
+      <c r="E34">
+        <v>140</v>
+      </c>
+      <c r="F34">
+        <v>140</v>
+      </c>
+      <c r="G34">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>90</v>
+      </c>
+      <c r="D35">
+        <v>90</v>
+      </c>
+      <c r="E35">
+        <v>80</v>
+      </c>
+      <c r="F35">
+        <v>120</v>
+      </c>
+      <c r="G35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>80</v>
+      </c>
+      <c r="D36">
+        <v>105</v>
+      </c>
+      <c r="E36">
+        <v>185</v>
+      </c>
+      <c r="F36">
+        <v>150</v>
+      </c>
+      <c r="G36">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>170</v>
+      </c>
+      <c r="D37">
+        <v>155</v>
+      </c>
+      <c r="E37">
+        <v>130</v>
+      </c>
+      <c r="F37">
+        <v>135</v>
+      </c>
+      <c r="G37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>155</v>
+      </c>
+      <c r="D38">
+        <v>70</v>
+      </c>
+      <c r="E38">
+        <v>60</v>
+      </c>
+      <c r="F38">
+        <v>50</v>
+      </c>
+      <c r="G38">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>100</v>
+      </c>
+      <c r="D39">
+        <v>135</v>
+      </c>
+      <c r="E39">
+        <v>95</v>
+      </c>
+      <c r="F39">
+        <v>100</v>
+      </c>
+      <c r="G39">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>115</v>
+      </c>
+      <c r="D40">
+        <v>130</v>
+      </c>
+      <c r="E40">
+        <v>125</v>
+      </c>
+      <c r="F40">
+        <v>105</v>
+      </c>
+      <c r="G40">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>120</v>
+      </c>
+      <c r="D41">
+        <v>60</v>
+      </c>
+      <c r="E41">
+        <v>110</v>
+      </c>
+      <c r="F41">
+        <v>75</v>
+      </c>
+      <c r="G41">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>125</v>
+      </c>
+      <c r="D42">
+        <v>110</v>
+      </c>
+      <c r="E42">
+        <v>110</v>
+      </c>
+      <c r="F42">
+        <v>120</v>
+      </c>
+      <c r="G42">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>125</v>
+      </c>
+      <c r="D43">
+        <v>150</v>
+      </c>
+      <c r="E43">
+        <v>130</v>
+      </c>
+      <c r="F43">
+        <v>150</v>
+      </c>
+      <c r="G43">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>75</v>
+      </c>
+      <c r="D44">
+        <v>85</v>
+      </c>
+      <c r="E44">
+        <v>85</v>
+      </c>
+      <c r="F44">
+        <v>90</v>
+      </c>
+      <c r="G44">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>145</v>
+      </c>
+      <c r="D45">
+        <v>90</v>
+      </c>
+      <c r="E45">
+        <v>60</v>
+      </c>
+      <c r="F45">
+        <v>105</v>
+      </c>
+      <c r="G45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>140</v>
+      </c>
+      <c r="D46">
+        <v>105</v>
+      </c>
+      <c r="E46">
+        <v>150</v>
+      </c>
+      <c r="F46">
+        <v>105</v>
+      </c>
+      <c r="G46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>150</v>
+      </c>
+      <c r="D47">
+        <v>155</v>
+      </c>
+      <c r="E47">
+        <v>165</v>
+      </c>
+      <c r="F47">
+        <v>140</v>
+      </c>
+      <c r="G47">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>140</v>
+      </c>
+      <c r="D48">
+        <v>140</v>
+      </c>
+      <c r="E48">
+        <v>135</v>
+      </c>
+      <c r="F48">
+        <v>80</v>
+      </c>
+      <c r="G48">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>95</v>
+      </c>
+      <c r="D49">
+        <v>95</v>
+      </c>
+      <c r="E49">
+        <v>115</v>
+      </c>
+      <c r="F49">
+        <v>65</v>
+      </c>
+      <c r="G49">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>110</v>
+      </c>
+      <c r="D50">
+        <v>85</v>
+      </c>
+      <c r="E50">
+        <v>135</v>
+      </c>
+      <c r="F50">
+        <v>110</v>
+      </c>
+      <c r="G50">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>115</v>
+      </c>
+      <c r="D51">
+        <v>95</v>
+      </c>
+      <c r="E51">
+        <v>140</v>
+      </c>
+      <c r="F51">
+        <v>95</v>
+      </c>
+      <c r="G51">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>95</v>
+      </c>
+      <c r="D52">
+        <v>95</v>
+      </c>
+      <c r="E52">
+        <v>50</v>
+      </c>
+      <c r="F52">
+        <v>110</v>
+      </c>
+      <c r="G52">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>85</v>
+      </c>
+      <c r="D53">
+        <v>125</v>
+      </c>
+      <c r="E53">
+        <v>145</v>
+      </c>
+      <c r="F53">
+        <v>110</v>
+      </c>
+      <c r="G53">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>145</v>
+      </c>
+      <c r="D54">
+        <v>130</v>
+      </c>
+      <c r="E54">
+        <v>100</v>
+      </c>
+      <c r="F54">
+        <v>95</v>
+      </c>
+      <c r="G54">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>50</v>
+      </c>
+      <c r="D55">
+        <v>85</v>
+      </c>
+      <c r="E55">
+        <v>80</v>
+      </c>
+      <c r="F55">
+        <v>70</v>
+      </c>
+      <c r="G55">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>85</v>
+      </c>
+      <c r="D56">
+        <v>85</v>
+      </c>
+      <c r="E56">
+        <v>115</v>
+      </c>
+      <c r="F56">
+        <v>105</v>
+      </c>
+      <c r="G56">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>135</v>
+      </c>
+      <c r="D57">
+        <v>80</v>
+      </c>
+      <c r="E57">
+        <v>75</v>
+      </c>
+      <c r="F57">
+        <v>130</v>
+      </c>
+      <c r="G57">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>95</v>
+      </c>
+      <c r="D58">
+        <v>140</v>
+      </c>
+      <c r="E58">
+        <v>125</v>
+      </c>
+      <c r="F58">
+        <v>110</v>
+      </c>
+      <c r="G58">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>100</v>
+      </c>
+      <c r="D59">
+        <v>110</v>
+      </c>
+      <c r="E59">
+        <v>100</v>
+      </c>
+      <c r="F59">
+        <v>80</v>
+      </c>
+      <c r="G59">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>140</v>
+      </c>
+      <c r="D60">
+        <v>100</v>
+      </c>
+      <c r="E60">
+        <v>105</v>
+      </c>
+      <c r="F60">
+        <v>85</v>
+      </c>
+      <c r="G60">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>115</v>
+      </c>
+      <c r="D61">
+        <v>120</v>
+      </c>
+      <c r="E61">
+        <v>115</v>
+      </c>
+      <c r="F61">
+        <v>125</v>
+      </c>
+      <c r="G61">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>95</v>
+      </c>
+      <c r="D62">
+        <v>90</v>
+      </c>
+      <c r="E62">
+        <v>100</v>
+      </c>
+      <c r="F62">
+        <v>135</v>
+      </c>
+      <c r="G62">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>145</v>
+      </c>
+      <c r="D63">
+        <v>135</v>
+      </c>
+      <c r="E63">
+        <v>125</v>
+      </c>
+      <c r="F63">
+        <v>120</v>
+      </c>
+      <c r="G63">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>